<commit_message>
hotfix: fixed find_element from umidade_atual
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -424,22 +424,22 @@
     <row r="2" ht="15" customHeight="1" s="8">
       <c r="A2" s="10" t="inlineStr">
         <is>
-          <t>22°C</t>
+          <t>23°C</t>
         </is>
       </c>
       <c r="B2" s="10" t="inlineStr">
         <is>
-          <t>77%</t>
+          <t>73%</t>
         </is>
       </c>
       <c r="C2" s="10" t="inlineStr">
         <is>
-          <t>20:03</t>
+          <t>15:30</t>
         </is>
       </c>
       <c r="D2" s="10" t="inlineStr">
         <is>
-          <t>segunda-feira, 10 de março</t>
+          <t>quarta-feira, 19 de março</t>
         </is>
       </c>
     </row>

</xml_diff>